<commit_message>
test: Add a row with Date object as value 'Birthday' in customers.xlsx
</commit_message>
<xml_diff>
--- a/cypress/fixtures/customers.xlsx
+++ b/cypress/fixtures/customers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -77,7 +77,10 @@
     <t xml:space="preserve">Beer</t>
   </si>
   <si>
-    <t xml:space="preserve">12/05/1987</t>
+    <t xml:space="preserve">21/05/2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billy</t>
   </si>
   <si>
     <t xml:space="preserve">This sheet should not be parsed when importing the file in the webapp</t>
@@ -90,9 +93,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -159,12 +164,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,17 +194,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -199,7 +212,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,6 +312,27 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>1.83</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <f aca="false">DATE(1940,4,28)</f>
+        <v>14729</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>
@@ -314,29 +347,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enable AgGrid column grouping, and add import/export in customToolbar
</commit_message>
<xml_diff>
--- a/cypress/fixtures/customers.xlsx
+++ b/cypress/fixtures/customers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -77,7 +77,10 @@
     <t xml:space="preserve">Beer</t>
   </si>
   <si>
-    <t xml:space="preserve">12/05/1987</t>
+    <t xml:space="preserve">21/05/2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billy</t>
   </si>
   <si>
     <t xml:space="preserve">This sheet should not be parsed when importing the file in the webapp</t>
@@ -90,9 +93,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -159,12 +164,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,17 +194,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -199,7 +212,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,6 +312,27 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>1.83</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <f aca="false">DATE(1940,4,28)</f>
+        <v>14729</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>
@@ -314,29 +347,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: [PROD-10305] implement add/delete row features
</commit_message>
<xml_diff>
--- a/cypress/fixtures/customers.xlsx
+++ b/cypress/fixtures/customers.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Beer</t>
   </si>
   <si>
-    <t xml:space="preserve">21/05/2002</t>
+    <t xml:space="preserve">12/05/1987</t>
   </si>
   <si>
     <t xml:space="preserve">Billy</t>
@@ -201,10 +201,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -321,7 +321,8 @@
       <c r="B6" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="b">
+      <c r="C6" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -357,7 +358,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>